<commit_message>
add dockerfile for render deployment
</commit_message>
<xml_diff>
--- a/test_history.xlsx
+++ b/test_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t>test_id</t>
   </si>
@@ -115,6 +115,9 @@
     <t>20260219_182506</t>
   </si>
   <si>
+    <t>20260219_184638</t>
+  </si>
+  <si>
     <t>2026-02-18 23:46:03</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
   </si>
   <si>
     <t>2026-02-19 18:25:06</t>
+  </si>
+  <si>
+    <t>2026-02-19 18:46:38</t>
   </si>
   <si>
     <t>open browser search for python tutorial</t>
@@ -226,6 +232,12 @@
                 search python playwright documentation</t>
   </si>
   <si>
+    <t>open browser go to https://www.youtube.com
+                search automation testing tutorial
+                wait 3000
+                click first video</t>
+  </si>
+  <si>
     <t>failed</t>
   </si>
   <si>
@@ -310,6 +322,9 @@
     <t>app/generated_tests\test_20260219_182433.py</t>
   </si>
   <si>
+    <t>app/generated_tests\test_20260219_184441.py</t>
+  </si>
+  <si>
     <t>test_logs/20260218_234603.json</t>
   </si>
   <si>
@@ -362,6 +377,9 @@
   </si>
   <si>
     <t>test_logs/20260219_182506.json</t>
+  </si>
+  <si>
+    <t>test_logs/20260219_184638.json</t>
   </si>
 </sst>
 </file>
@@ -732,7 +750,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -790,10 +808,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -811,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -820,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -831,10 +849,10 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -852,22 +870,22 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -875,13 +893,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -896,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -905,10 +923,10 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -916,13 +934,13 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -937,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -946,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="O5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -957,10 +975,10 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -978,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -987,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="O6" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -998,13 +1016,13 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1019,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -1028,10 +1046,10 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1039,13 +1057,13 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1060,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -1069,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="O8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1080,10 +1098,10 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1101,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -1110,10 +1128,10 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O9" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1121,10 +1139,10 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -1142,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -1151,10 +1169,10 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O10" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1162,13 +1180,13 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1183,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -1192,10 +1210,10 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="O11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1203,13 +1221,13 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1224,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -1233,10 +1251,10 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="O12" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1244,10 +1262,10 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -1265,22 +1283,22 @@
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="O13" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1288,13 +1306,13 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1309,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -1318,10 +1336,10 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="O14" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1329,10 +1347,10 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1350,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -1359,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="O15" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1370,10 +1388,10 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1391,7 +1409,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -1400,10 +1418,10 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="O16" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1411,13 +1429,13 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1432,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -1441,10 +1459,10 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O17" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1452,10 +1470,10 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1473,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1482,10 +1500,10 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="O18" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1493,13 +1511,13 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1514,22 +1532,63 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>93</v>
+      </c>
+      <c r="O19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
         <v>66</v>
       </c>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>90</v>
-      </c>
-      <c r="O19" t="s">
-        <v>108</v>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>94</v>
+      </c>
+      <c r="O20" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1552,6 +1611,7 @@
     <hyperlink ref="I17" r:id="rId16"/>
     <hyperlink ref="I18" r:id="rId17"/>
     <hyperlink ref="I19" r:id="rId18"/>
+    <hyperlink ref="I20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>